<commit_message>
RS232 & Powder List
</commit_message>
<xml_diff>
--- a/Hardware/RS232/JLCSMT_CPL.xlsx
+++ b/Hardware/RS232/JLCSMT_CPL.xlsx
@@ -214,7 +214,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13:E13"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -302,7 +302,7 @@
         <v>21.75</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>15.24</v>
+        <v>14.84</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>6</v>

</xml_diff>